<commit_message>
chose(Auto eval) : ajout de l'auto eval et mise à jour de jnr
</commit_message>
<xml_diff>
--- a/m-planification-jnltrav.xlsx
+++ b/m-planification-jnltrav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Module I320\Administratif\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P_OO-Shoot-me-up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB41038-7BB2-415F-A5C9-C966BBB41193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB852DD-8CE4-47C5-9D17-C75F3F19F241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>J'ai créer les User story de mon projet</t>
+  </si>
+  <si>
+    <t>Feet back du livrable de vendredi dernier</t>
   </si>
 </sst>
 </file>
@@ -805,11 +808,11 @@
   </sheetPr>
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1020,13 +1023,19 @@
       <c r="E17" s="32"/>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B18" s="27">
         <f>B12+7</f>
         <v>45910</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="5">
+        <v>25</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1402,7 +1411,7 @@
       <c r="B66" s="34"/>
       <c r="C66" s="15">
         <f>MROUND(SUM(C6:C65) /60,0.2)</f>
-        <v>4.6000000000000005</v>
+        <v>5</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="17"/>

</xml_diff>